<commit_message>
Updating sorting order check for utilitysummary
</commit_message>
<xml_diff>
--- a/Testdata/UtilityOutcome_QOL_Data_Staging.xlsx
+++ b/Testdata/UtilityOutcome_QOL_Data_Staging.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C767B58E-FC55-4AC6-9209-4F821BB6A512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95135F43-D227-45D4-8C49-78F0B2DD892A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewImportLogic" sheetId="1" r:id="rId1"/>
     <sheet name="OldImportLogic" sheetId="2" r:id="rId2"/>
+    <sheet name="prodfix" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
   <si>
     <t>Population</t>
   </si>
@@ -111,6 +112,57 @@
   </si>
   <si>
     <t>\Testdata\Templates\UtilityOutcome\QOL_ECON_Staging\OldImportLogic\QOL_OldImportExpectedResult.xlsx</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Import_Pop</t>
+  </si>
+  <si>
+    <t>ExtractionFile</t>
+  </si>
+  <si>
+    <t>scenario1</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\UtilityOutcome\QOL_ECON_Staging\PROD_Fix\UtilityOutcome_Feature_Extraction_file_ExpectedData.xlsx</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\UtilityOutcome\QOL_ECON_Staging\PROD_Fix\Templates\UtilityOutcome_Feature_Extraction_file_QoL_UtilityData_ECON_NoUtility.xlsx</t>
+  </si>
+  <si>
+    <t>scenario2</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\UtilityOutcome\QOL_ECON_Staging\PROD_Fix\Templates\UtilityOutcome_Feature_Extraction_file_ECON_UtilityData_QoL_NoUtility.xlsx</t>
+  </si>
+  <si>
+    <t>scenario3</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\UtilityOutcome\QOL_ECON_Staging\PROD_Fix\Templates\UtilityOutcome_Feature_Extraction_file_Both_QoL_ECON_Utility.xlsx</t>
+  </si>
+  <si>
+    <t>scenario4</t>
+  </si>
+  <si>
+    <t>\Testdata\Templates\UtilityOutcome\QOL_ECON_Staging\PROD_Fix\Templates\UtilityOutcome_Feature_Extraction_file_NegativeScenario_QoL__ECON_NoUtility.xlsx</t>
+  </si>
+  <si>
+    <t>PRODFix_QOL_ECON - UtilityOutcome</t>
+  </si>
+  <si>
+    <t>PRODFix_QOL_ECON - UtilityOutcome_radio_button</t>
+  </si>
+  <si>
+    <t>UtilityOutcome - PRODFix_QOL_ECON - Ovid search - 9/19/2022</t>
+  </si>
+  <si>
+    <t>ExcelReport-PRODFix_QOL_ECON - UtilityOutcome-Quality of Life-</t>
+  </si>
+  <si>
+    <t>WordReport-PRODFix_QOL_ECON - UtilityOutcome-Quality of Life-</t>
   </si>
 </sst>
 </file>
@@ -430,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DACE520-ADCB-4DB7-8DF5-26FC52F0DAE9}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -612,4 +664,250 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84D6FF7-55D3-4D63-AD07-5FB8EC80054E}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" customWidth="1"/>
+    <col min="8" max="8" width="27.77734375" customWidth="1"/>
+    <col min="9" max="9" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>